<commit_message>
Update reports and lists
</commit_message>
<xml_diff>
--- a/inferences/paises_totais_n.xlsx
+++ b/inferences/paises_totais_n.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>